<commit_message>
Updated file names. Updated templates and screenshots.
</commit_message>
<xml_diff>
--- a/_templates/Strategic-Logistics-Board/Warehouse_Complaints_en.xlsx
+++ b/_templates/Strategic-Logistics-Board/Warehouse_Complaints_en.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Strategic_Logistics_Board/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Strategic-Logistics-Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BCCDFA-1123-7B49-8234-EBEAE407DE31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AD344F-3937-B843-96F0-617681CD01A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-52000" yWindow="-3720" windowWidth="42920" windowHeight="28080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="225">
   <si>
     <t>date</t>
   </si>
@@ -46,15 +46,9 @@
     <t>12:23:43</t>
   </si>
   <si>
-    <t>Damaged package</t>
-  </si>
-  <si>
     <t>16:31:21</t>
   </si>
   <si>
-    <t>Too late</t>
-  </si>
-  <si>
     <t>4:47:22</t>
   </si>
   <si>
@@ -676,10 +670,34 @@
     <t>Don't forget the Apples.</t>
   </si>
   <si>
-    <t>Half order came in time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2 of 3 types were incomplete</t>
+    <t>Damaged Packaging</t>
+  </si>
+  <si>
+    <t>Delayed</t>
+  </si>
+  <si>
+    <t>It was delivered in the wrong order. Was hard to find the right parts afterwards.</t>
+  </si>
+  <si>
+    <t>The package was damaged on one side. Content was ok.</t>
+  </si>
+  <si>
+    <t>The delivery was needed already on Monday.</t>
+  </si>
+  <si>
+    <t>Only 4 of 8 wine were delivered.</t>
+  </si>
+  <si>
+    <t>Only half the order came in time.</t>
+  </si>
+  <si>
+    <t>Apples were not delivered.</t>
+  </si>
+  <si>
+    <t>Please keep an eye on the little things. 2 out of 3 items were incomplete.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 out of 3 items were incomplete.</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1051,7 @@
   <dimension ref="A1:E200"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1053,7 +1071,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1076,7 +1094,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -1090,10 +1108,10 @@
         <v>300</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E3" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -1101,16 +1119,16 @@
         <v>43759</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>200</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E4" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -1118,16 +1136,16 @@
         <v>43758</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>400</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -1135,16 +1153,16 @@
         <v>43757</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E6" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -1152,16 +1170,16 @@
         <v>43756</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>400</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -1169,16 +1187,16 @@
         <v>43755</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>400</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -1186,16 +1204,16 @@
         <v>43754</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>300</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -1203,16 +1221,16 @@
         <v>43753</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>400</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -1220,16 +1238,16 @@
         <v>43752</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>400</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -1237,16 +1255,16 @@
         <v>43751</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>300</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -1254,16 +1272,16 @@
         <v>43750</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>400</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -1271,16 +1289,16 @@
         <v>43749</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>300</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -1288,16 +1306,16 @@
         <v>43748</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>400</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
@@ -1305,7 +1323,7 @@
         <v>43747</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <v>100</v>
@@ -1314,7 +1332,7 @@
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -1322,16 +1340,16 @@
         <v>43746</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>400</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
@@ -1339,7 +1357,7 @@
         <v>43745</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18">
         <v>100</v>
@@ -1348,7 +1366,7 @@
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
@@ -1356,16 +1374,16 @@
         <v>43744</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19">
         <v>200</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -1373,16 +1391,16 @@
         <v>43743</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20">
         <v>400</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
@@ -1390,16 +1408,16 @@
         <v>43742</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21">
         <v>400</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -1407,16 +1425,16 @@
         <v>43741</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C22">
         <v>400</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
@@ -1424,16 +1442,16 @@
         <v>43740</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C23">
         <v>400</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
@@ -1441,7 +1459,7 @@
         <v>43739</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C24">
         <v>100</v>
@@ -1450,7 +1468,7 @@
         <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
@@ -1458,16 +1476,16 @@
         <v>43738</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C25">
         <v>300</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E25" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
@@ -1475,7 +1493,7 @@
         <v>43737</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26">
         <v>100</v>
@@ -1484,7 +1502,7 @@
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
@@ -1492,16 +1510,16 @@
         <v>43736</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C27">
         <v>200</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E27" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
@@ -1509,16 +1527,16 @@
         <v>43735</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C28">
         <v>400</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
@@ -1526,16 +1544,16 @@
         <v>43734</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C29">
         <v>400</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
@@ -1543,16 +1561,16 @@
         <v>43733</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C30">
         <v>400</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
@@ -1560,16 +1578,16 @@
         <v>43732</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C31">
         <v>300</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E31" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
@@ -1577,16 +1595,16 @@
         <v>43731</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C32">
         <v>200</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E32" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
@@ -1594,16 +1612,16 @@
         <v>43730</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C33">
         <v>300</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E33" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
@@ -1611,16 +1629,16 @@
         <v>43729</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C34">
         <v>400</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E34" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
@@ -1628,16 +1646,16 @@
         <v>43728</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C35">
         <v>400</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
@@ -1645,16 +1663,16 @@
         <v>43727</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C36">
         <v>400</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E36" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
@@ -1662,16 +1680,16 @@
         <v>43726</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C37">
         <v>400</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
@@ -1679,16 +1697,16 @@
         <v>43725</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C38">
         <v>400</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E38" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
@@ -1696,16 +1714,16 @@
         <v>43724</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C39">
         <v>400</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
@@ -1713,16 +1731,16 @@
         <v>43723</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C40">
         <v>200</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E40" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
@@ -1730,16 +1748,16 @@
         <v>43722</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C41">
         <v>400</v>
       </c>
       <c r="D41" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
@@ -1747,16 +1765,16 @@
         <v>43721</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C42">
         <v>400</v>
       </c>
       <c r="D42" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
@@ -1764,16 +1782,16 @@
         <v>43720</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C43">
         <v>400</v>
       </c>
       <c r="D43" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E43" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
@@ -1781,16 +1799,16 @@
         <v>43719</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C44">
         <v>200</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E44" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
@@ -1798,16 +1816,16 @@
         <v>43718</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C45">
         <v>300</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E45" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
@@ -1815,7 +1833,7 @@
         <v>43717</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C46">
         <v>100</v>
@@ -1824,7 +1842,7 @@
         <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
@@ -1832,16 +1850,16 @@
         <v>43716</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C47">
         <v>200</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E47" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
@@ -1849,16 +1867,16 @@
         <v>43715</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C48">
         <v>400</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
@@ -1866,16 +1884,16 @@
         <v>43714</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C49">
         <v>400</v>
       </c>
       <c r="D49" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E49" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
@@ -1883,16 +1901,16 @@
         <v>43713</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C50">
         <v>200</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E50" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
@@ -1900,16 +1918,16 @@
         <v>43712</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C51">
         <v>400</v>
       </c>
       <c r="D51" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E51" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
@@ -1917,16 +1935,16 @@
         <v>43711</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C52">
         <v>400</v>
       </c>
       <c r="D52" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E52" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
@@ -1934,16 +1952,16 @@
         <v>43710</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C53">
         <v>400</v>
       </c>
       <c r="D53" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E53" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
@@ -1951,16 +1969,16 @@
         <v>43709</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C54">
         <v>300</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E54" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
@@ -1968,16 +1986,16 @@
         <v>43708</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C55">
         <v>400</v>
       </c>
       <c r="D55" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E55" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
@@ -1985,16 +2003,16 @@
         <v>43707</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C56">
         <v>400</v>
       </c>
       <c r="D56" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E56" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
@@ -2002,16 +2020,16 @@
         <v>43706</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C57">
         <v>400</v>
       </c>
       <c r="D57" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E57" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
@@ -2019,16 +2037,16 @@
         <v>43705</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C58">
         <v>300</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E58" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
@@ -2036,16 +2054,16 @@
         <v>43704</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C59">
         <v>400</v>
       </c>
       <c r="D59" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E59" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
@@ -2053,16 +2071,16 @@
         <v>43703</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C60">
         <v>400</v>
       </c>
       <c r="D60" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E60" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
@@ -2070,16 +2088,16 @@
         <v>43702</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C61">
         <v>400</v>
       </c>
       <c r="D61" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E61" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
@@ -2087,16 +2105,16 @@
         <v>43701</v>
       </c>
       <c r="B62" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C62">
         <v>400</v>
       </c>
       <c r="D62" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E62" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
@@ -2104,16 +2122,16 @@
         <v>43700</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C63">
         <v>200</v>
       </c>
       <c r="D63" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E63" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
@@ -2121,16 +2139,16 @@
         <v>43699</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C64">
         <v>400</v>
       </c>
       <c r="D64" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E64" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
@@ -2138,16 +2156,16 @@
         <v>43698</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C65">
         <v>400</v>
       </c>
       <c r="D65" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E65" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
@@ -2155,16 +2173,16 @@
         <v>43697</v>
       </c>
       <c r="B66" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C66">
         <v>300</v>
       </c>
       <c r="D66" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E66" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
@@ -2172,16 +2190,16 @@
         <v>43696</v>
       </c>
       <c r="B67" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C67">
         <v>400</v>
       </c>
       <c r="D67" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E67" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
@@ -2189,16 +2207,16 @@
         <v>43695</v>
       </c>
       <c r="B68" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C68">
         <v>200</v>
       </c>
       <c r="D68" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E68" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
@@ -2206,16 +2224,16 @@
         <v>43694</v>
       </c>
       <c r="B69" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C69">
         <v>400</v>
       </c>
       <c r="D69" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E69" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
@@ -2223,16 +2241,16 @@
         <v>43693</v>
       </c>
       <c r="B70" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C70">
         <v>300</v>
       </c>
       <c r="D70" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E70" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
@@ -2240,16 +2258,16 @@
         <v>43692</v>
       </c>
       <c r="B71" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C71">
         <v>400</v>
       </c>
       <c r="D71" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E71" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
@@ -2257,16 +2275,16 @@
         <v>43691</v>
       </c>
       <c r="B72" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C72">
         <v>400</v>
       </c>
       <c r="D72" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E72" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
@@ -2274,16 +2292,16 @@
         <v>43690</v>
       </c>
       <c r="B73" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C73">
         <v>400</v>
       </c>
       <c r="D73" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E73" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
@@ -2291,16 +2309,16 @@
         <v>43689</v>
       </c>
       <c r="B74" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C74">
         <v>300</v>
       </c>
       <c r="D74" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E74" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
@@ -2308,16 +2326,16 @@
         <v>43688</v>
       </c>
       <c r="B75" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C75">
         <v>200</v>
       </c>
       <c r="D75" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E75" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
@@ -2325,16 +2343,16 @@
         <v>43687</v>
       </c>
       <c r="B76" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C76">
         <v>400</v>
       </c>
       <c r="D76" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E76" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
@@ -2342,16 +2360,16 @@
         <v>43686</v>
       </c>
       <c r="B77" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C77">
         <v>200</v>
       </c>
       <c r="D77" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E77" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
@@ -2359,16 +2377,16 @@
         <v>43685</v>
       </c>
       <c r="B78" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C78">
         <v>400</v>
       </c>
       <c r="D78" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E78" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
@@ -2376,16 +2394,16 @@
         <v>43684</v>
       </c>
       <c r="B79" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C79">
         <v>300</v>
       </c>
       <c r="D79" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E79" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
@@ -2393,16 +2411,16 @@
         <v>43683</v>
       </c>
       <c r="B80" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C80">
         <v>200</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E80" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
@@ -2410,16 +2428,16 @@
         <v>43682</v>
       </c>
       <c r="B81" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C81">
         <v>400</v>
       </c>
       <c r="D81" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E81" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
@@ -2427,16 +2445,16 @@
         <v>43681</v>
       </c>
       <c r="B82" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C82">
         <v>400</v>
       </c>
       <c r="D82" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E82" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
@@ -2444,16 +2462,16 @@
         <v>43680</v>
       </c>
       <c r="B83" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C83">
         <v>300</v>
       </c>
       <c r="D83" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E83" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
@@ -2461,16 +2479,16 @@
         <v>43679</v>
       </c>
       <c r="B84" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C84">
         <v>400</v>
       </c>
       <c r="D84" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E84" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
@@ -2478,16 +2496,16 @@
         <v>43678</v>
       </c>
       <c r="B85" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C85">
         <v>400</v>
       </c>
       <c r="D85" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E85" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
@@ -2495,16 +2513,16 @@
         <v>43677</v>
       </c>
       <c r="B86" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C86">
         <v>400</v>
       </c>
       <c r="D86" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E86" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.15">
@@ -2512,16 +2530,16 @@
         <v>43676</v>
       </c>
       <c r="B87" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C87">
         <v>400</v>
       </c>
       <c r="D87" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E87" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.15">
@@ -2529,16 +2547,16 @@
         <v>43675</v>
       </c>
       <c r="B88" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C88">
         <v>200</v>
       </c>
       <c r="D88" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E88" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.15">
@@ -2546,16 +2564,16 @@
         <v>43674</v>
       </c>
       <c r="B89" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C89">
         <v>400</v>
       </c>
       <c r="D89" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E89" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.15">
@@ -2563,16 +2581,16 @@
         <v>43673</v>
       </c>
       <c r="B90" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C90">
         <v>200</v>
       </c>
       <c r="D90" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E90" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.15">
@@ -2580,16 +2598,16 @@
         <v>43672</v>
       </c>
       <c r="B91" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C91">
         <v>400</v>
       </c>
       <c r="D91" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E91" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
@@ -2597,16 +2615,16 @@
         <v>43671</v>
       </c>
       <c r="B92" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C92">
         <v>400</v>
       </c>
       <c r="D92" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E92" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
@@ -2614,16 +2632,16 @@
         <v>43670</v>
       </c>
       <c r="B93" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C93">
         <v>400</v>
       </c>
       <c r="D93" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E93" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.15">
@@ -2631,16 +2649,16 @@
         <v>43669</v>
       </c>
       <c r="B94" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C94">
         <v>200</v>
       </c>
       <c r="D94" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E94" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.15">
@@ -2648,16 +2666,16 @@
         <v>43668</v>
       </c>
       <c r="B95" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C95">
         <v>400</v>
       </c>
       <c r="D95" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E95" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.15">
@@ -2665,16 +2683,16 @@
         <v>43667</v>
       </c>
       <c r="B96" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C96">
         <v>400</v>
       </c>
       <c r="D96" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E96" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.15">
@@ -2682,16 +2700,16 @@
         <v>43666</v>
       </c>
       <c r="B97" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C97">
         <v>400</v>
       </c>
       <c r="D97" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E97" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.15">
@@ -2699,16 +2717,16 @@
         <v>43665</v>
       </c>
       <c r="B98" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C98">
         <v>200</v>
       </c>
       <c r="D98" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E98" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.15">
@@ -2716,7 +2734,7 @@
         <v>43664</v>
       </c>
       <c r="B99" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C99">
         <v>100</v>
@@ -2725,7 +2743,7 @@
         <v>5</v>
       </c>
       <c r="E99" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.15">
@@ -2733,16 +2751,16 @@
         <v>43663</v>
       </c>
       <c r="B100" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C100">
         <v>300</v>
       </c>
       <c r="D100" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E100" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.15">
@@ -2750,16 +2768,16 @@
         <v>43662</v>
       </c>
       <c r="B101" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C101">
         <v>400</v>
       </c>
       <c r="D101" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E101" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.15">
@@ -2767,7 +2785,7 @@
         <v>43661</v>
       </c>
       <c r="B102" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C102">
         <v>100</v>
@@ -2776,7 +2794,7 @@
         <v>5</v>
       </c>
       <c r="E102" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.15">
@@ -2784,16 +2802,16 @@
         <v>43660</v>
       </c>
       <c r="B103" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C103">
         <v>300</v>
       </c>
       <c r="D103" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E103" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.15">
@@ -2801,16 +2819,16 @@
         <v>43659</v>
       </c>
       <c r="B104" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C104">
         <v>300</v>
       </c>
       <c r="D104" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E104" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.15">
@@ -2818,16 +2836,16 @@
         <v>43658</v>
       </c>
       <c r="B105" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C105">
         <v>400</v>
       </c>
       <c r="D105" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E105" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.15">
@@ -2835,16 +2853,16 @@
         <v>43657</v>
       </c>
       <c r="B106" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C106">
         <v>300</v>
       </c>
       <c r="D106" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E106" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.15">
@@ -2852,7 +2870,7 @@
         <v>43656</v>
       </c>
       <c r="B107" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C107">
         <v>100</v>
@@ -2861,7 +2879,7 @@
         <v>5</v>
       </c>
       <c r="E107" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.15">
@@ -2869,7 +2887,7 @@
         <v>43655</v>
       </c>
       <c r="B108" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C108">
         <v>100</v>
@@ -2878,7 +2896,7 @@
         <v>5</v>
       </c>
       <c r="E108" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.15">
@@ -2886,7 +2904,7 @@
         <v>43654</v>
       </c>
       <c r="B109" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C109">
         <v>100</v>
@@ -2895,7 +2913,7 @@
         <v>5</v>
       </c>
       <c r="E109" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.15">
@@ -2903,16 +2921,16 @@
         <v>43653</v>
       </c>
       <c r="B110" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C110">
         <v>200</v>
       </c>
       <c r="D110" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E110" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.15">
@@ -2920,16 +2938,16 @@
         <v>43652</v>
       </c>
       <c r="B111" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C111">
         <v>300</v>
       </c>
       <c r="D111" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E111" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.15">
@@ -2937,16 +2955,16 @@
         <v>43651</v>
       </c>
       <c r="B112" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C112">
         <v>300</v>
       </c>
       <c r="D112" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E112" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.15">
@@ -2954,16 +2972,16 @@
         <v>43650</v>
       </c>
       <c r="B113" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C113">
         <v>300</v>
       </c>
       <c r="D113" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E113" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.15">
@@ -2971,7 +2989,7 @@
         <v>43649</v>
       </c>
       <c r="B114" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C114">
         <v>100</v>
@@ -2980,7 +2998,7 @@
         <v>5</v>
       </c>
       <c r="E114" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.15">
@@ -2988,16 +3006,16 @@
         <v>43648</v>
       </c>
       <c r="B115" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C115">
         <v>300</v>
       </c>
       <c r="D115" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E115" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.15">
@@ -3005,16 +3023,16 @@
         <v>43647</v>
       </c>
       <c r="B116" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C116">
         <v>400</v>
       </c>
       <c r="D116" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E116" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.15">
@@ -3022,16 +3040,16 @@
         <v>43646</v>
       </c>
       <c r="B117" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C117">
         <v>400</v>
       </c>
       <c r="D117" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E117" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.15">
@@ -3039,16 +3057,16 @@
         <v>43645</v>
       </c>
       <c r="B118" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C118">
         <v>400</v>
       </c>
       <c r="D118" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E118" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.15">
@@ -3056,16 +3074,16 @@
         <v>43644</v>
       </c>
       <c r="B119" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C119">
         <v>400</v>
       </c>
       <c r="D119" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E119" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.15">
@@ -3073,16 +3091,16 @@
         <v>43643</v>
       </c>
       <c r="B120" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C120">
         <v>200</v>
       </c>
       <c r="D120" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E120" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.15">
@@ -3090,16 +3108,16 @@
         <v>43642</v>
       </c>
       <c r="B121" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C121">
         <v>400</v>
       </c>
       <c r="D121" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E121" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.15">
@@ -3107,16 +3125,16 @@
         <v>43641</v>
       </c>
       <c r="B122" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C122">
         <v>400</v>
       </c>
       <c r="D122" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E122" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.15">
@@ -3124,16 +3142,16 @@
         <v>43640</v>
       </c>
       <c r="B123" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C123">
         <v>200</v>
       </c>
       <c r="D123" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E123" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.15">
@@ -3141,7 +3159,7 @@
         <v>43639</v>
       </c>
       <c r="B124" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C124">
         <v>100</v>
@@ -3150,7 +3168,7 @@
         <v>5</v>
       </c>
       <c r="E124" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.15">
@@ -3158,16 +3176,16 @@
         <v>43638</v>
       </c>
       <c r="B125" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C125">
         <v>200</v>
       </c>
       <c r="D125" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E125" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.15">
@@ -3175,16 +3193,16 @@
         <v>43637</v>
       </c>
       <c r="B126" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C126">
         <v>200</v>
       </c>
       <c r="D126" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E126" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.15">
@@ -3192,7 +3210,7 @@
         <v>43636</v>
       </c>
       <c r="B127" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C127">
         <v>100</v>
@@ -3201,7 +3219,7 @@
         <v>5</v>
       </c>
       <c r="E127" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.15">
@@ -3209,16 +3227,16 @@
         <v>43635</v>
       </c>
       <c r="B128" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C128">
         <v>300</v>
       </c>
       <c r="D128" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E128" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.15">
@@ -3226,16 +3244,16 @@
         <v>43634</v>
       </c>
       <c r="B129" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C129">
         <v>200</v>
       </c>
       <c r="D129" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E129" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.15">
@@ -3243,16 +3261,16 @@
         <v>43633</v>
       </c>
       <c r="B130" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C130">
         <v>300</v>
       </c>
       <c r="D130" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E130" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.15">
@@ -3260,16 +3278,16 @@
         <v>43632</v>
       </c>
       <c r="B131" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C131">
         <v>300</v>
       </c>
       <c r="D131" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E131" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.15">
@@ -3277,16 +3295,16 @@
         <v>43631</v>
       </c>
       <c r="B132" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C132">
         <v>400</v>
       </c>
       <c r="D132" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E132" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.15">
@@ -3294,16 +3312,16 @@
         <v>43630</v>
       </c>
       <c r="B133" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C133">
         <v>300</v>
       </c>
       <c r="D133" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E133" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.15">
@@ -3311,7 +3329,7 @@
         <v>43629</v>
       </c>
       <c r="B134" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C134">
         <v>100</v>
@@ -3320,7 +3338,7 @@
         <v>5</v>
       </c>
       <c r="E134" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.15">
@@ -3328,7 +3346,7 @@
         <v>43628</v>
       </c>
       <c r="B135" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C135">
         <v>100</v>
@@ -3337,7 +3355,7 @@
         <v>5</v>
       </c>
       <c r="E135" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.15">
@@ -3345,16 +3363,16 @@
         <v>43627</v>
       </c>
       <c r="B136" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C136">
         <v>400</v>
       </c>
       <c r="D136" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E136" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.15">
@@ -3362,16 +3380,16 @@
         <v>43626</v>
       </c>
       <c r="B137" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C137">
         <v>400</v>
       </c>
       <c r="D137" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E137" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.15">
@@ -3379,16 +3397,16 @@
         <v>43625</v>
       </c>
       <c r="B138" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C138">
         <v>200</v>
       </c>
       <c r="D138" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E138" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.15">
@@ -3396,7 +3414,7 @@
         <v>43624</v>
       </c>
       <c r="B139" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C139">
         <v>100</v>
@@ -3405,7 +3423,7 @@
         <v>5</v>
       </c>
       <c r="E139" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.15">
@@ -3413,7 +3431,7 @@
         <v>43623</v>
       </c>
       <c r="B140" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C140">
         <v>100</v>
@@ -3422,7 +3440,7 @@
         <v>5</v>
       </c>
       <c r="E140" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.15">
@@ -3430,7 +3448,7 @@
         <v>43622</v>
       </c>
       <c r="B141" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C141">
         <v>100</v>
@@ -3439,7 +3457,7 @@
         <v>5</v>
       </c>
       <c r="E141" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.15">
@@ -3447,16 +3465,16 @@
         <v>43621</v>
       </c>
       <c r="B142" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C142">
         <v>200</v>
       </c>
       <c r="D142" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E142" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.15">
@@ -3464,16 +3482,16 @@
         <v>43620</v>
       </c>
       <c r="B143" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C143">
         <v>400</v>
       </c>
       <c r="D143" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E143" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.15">
@@ -3481,16 +3499,16 @@
         <v>43619</v>
       </c>
       <c r="B144" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C144">
         <v>200</v>
       </c>
       <c r="D144" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E144" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.15">
@@ -3498,16 +3516,16 @@
         <v>43618</v>
       </c>
       <c r="B145" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C145">
         <v>200</v>
       </c>
       <c r="D145" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E145" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.15">
@@ -3515,7 +3533,7 @@
         <v>43617</v>
       </c>
       <c r="B146" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C146">
         <v>100</v>
@@ -3524,7 +3542,7 @@
         <v>5</v>
       </c>
       <c r="E146" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.15">
@@ -3532,16 +3550,16 @@
         <v>43616</v>
       </c>
       <c r="B147" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C147">
         <v>200</v>
       </c>
       <c r="D147" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E147" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.15">
@@ -3549,16 +3567,16 @@
         <v>43615</v>
       </c>
       <c r="B148" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C148">
         <v>300</v>
       </c>
       <c r="D148" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E148" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.15">
@@ -3566,16 +3584,16 @@
         <v>43614</v>
       </c>
       <c r="B149" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C149">
         <v>400</v>
       </c>
       <c r="D149" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E149" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.15">
@@ -3583,16 +3601,16 @@
         <v>43613</v>
       </c>
       <c r="B150" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C150">
         <v>400</v>
       </c>
       <c r="D150" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E150" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.15">
@@ -3600,16 +3618,16 @@
         <v>43612</v>
       </c>
       <c r="B151" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C151">
         <v>400</v>
       </c>
       <c r="D151" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E151" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.15">
@@ -3617,16 +3635,16 @@
         <v>43611</v>
       </c>
       <c r="B152" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C152">
         <v>300</v>
       </c>
       <c r="D152" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E152" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.15">
@@ -3634,16 +3652,16 @@
         <v>43610</v>
       </c>
       <c r="B153" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C153">
         <v>400</v>
       </c>
       <c r="D153" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E153" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.15">
@@ -3651,16 +3669,16 @@
         <v>43609</v>
       </c>
       <c r="B154" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C154">
         <v>300</v>
       </c>
       <c r="D154" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E154" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.15">
@@ -3668,16 +3686,16 @@
         <v>43608</v>
       </c>
       <c r="B155" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C155">
         <v>300</v>
       </c>
       <c r="D155" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E155" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.15">
@@ -3685,16 +3703,16 @@
         <v>43607</v>
       </c>
       <c r="B156" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C156">
         <v>300</v>
       </c>
       <c r="D156" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E156" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.15">
@@ -3702,16 +3720,16 @@
         <v>43606</v>
       </c>
       <c r="B157" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C157">
         <v>200</v>
       </c>
       <c r="D157" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E157" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.15">
@@ -3719,7 +3737,7 @@
         <v>43605</v>
       </c>
       <c r="B158" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C158">
         <v>100</v>
@@ -3728,7 +3746,7 @@
         <v>5</v>
       </c>
       <c r="E158" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.15">
@@ -3736,7 +3754,7 @@
         <v>43604</v>
       </c>
       <c r="B159" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C159">
         <v>100</v>
@@ -3745,7 +3763,7 @@
         <v>5</v>
       </c>
       <c r="E159" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.15">
@@ -3753,16 +3771,16 @@
         <v>43603</v>
       </c>
       <c r="B160" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C160">
         <v>200</v>
       </c>
       <c r="D160" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E160" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.15">
@@ -3770,16 +3788,16 @@
         <v>43602</v>
       </c>
       <c r="B161" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C161">
         <v>400</v>
       </c>
       <c r="D161" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E161" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.15">
@@ -3787,7 +3805,7 @@
         <v>43601</v>
       </c>
       <c r="B162" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C162">
         <v>100</v>
@@ -3796,7 +3814,7 @@
         <v>5</v>
       </c>
       <c r="E162" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.15">
@@ -3804,7 +3822,7 @@
         <v>43600</v>
       </c>
       <c r="B163" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C163">
         <v>100</v>
@@ -3813,7 +3831,7 @@
         <v>5</v>
       </c>
       <c r="E163" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.15">
@@ -3821,7 +3839,7 @@
         <v>43599</v>
       </c>
       <c r="B164" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C164">
         <v>100</v>
@@ -3830,7 +3848,7 @@
         <v>5</v>
       </c>
       <c r="E164" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.15">
@@ -3838,16 +3856,16 @@
         <v>43598</v>
       </c>
       <c r="B165" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C165">
         <v>200</v>
       </c>
       <c r="D165" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E165" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.15">
@@ -3855,7 +3873,7 @@
         <v>43597</v>
       </c>
       <c r="B166" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C166">
         <v>100</v>
@@ -3864,7 +3882,7 @@
         <v>5</v>
       </c>
       <c r="E166" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.15">
@@ -3872,16 +3890,16 @@
         <v>43596</v>
       </c>
       <c r="B167" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C167">
         <v>200</v>
       </c>
       <c r="D167" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E167" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.15">
@@ -3889,7 +3907,7 @@
         <v>43595</v>
       </c>
       <c r="B168" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C168">
         <v>100</v>
@@ -3898,7 +3916,7 @@
         <v>5</v>
       </c>
       <c r="E168" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.15">
@@ -3906,16 +3924,16 @@
         <v>43594</v>
       </c>
       <c r="B169" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C169">
         <v>300</v>
       </c>
       <c r="D169" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E169" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.15">
@@ -3923,16 +3941,16 @@
         <v>43593</v>
       </c>
       <c r="B170" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C170">
         <v>300</v>
       </c>
       <c r="D170" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E170" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.15">
@@ -3940,7 +3958,7 @@
         <v>43592</v>
       </c>
       <c r="B171" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C171">
         <v>100</v>
@@ -3949,7 +3967,7 @@
         <v>5</v>
       </c>
       <c r="E171" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.15">
@@ -3957,7 +3975,7 @@
         <v>43591</v>
       </c>
       <c r="B172" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C172">
         <v>100</v>
@@ -3966,7 +3984,7 @@
         <v>5</v>
       </c>
       <c r="E172" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.15">
@@ -3974,16 +3992,16 @@
         <v>43590</v>
       </c>
       <c r="B173" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C173">
         <v>200</v>
       </c>
       <c r="D173" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E173" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.15">
@@ -3991,7 +4009,7 @@
         <v>43589</v>
       </c>
       <c r="B174" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C174">
         <v>100</v>
@@ -4000,7 +4018,7 @@
         <v>5</v>
       </c>
       <c r="E174" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.15">
@@ -4008,16 +4026,16 @@
         <v>43588</v>
       </c>
       <c r="B175" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C175">
         <v>400</v>
       </c>
       <c r="D175" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E175" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.15">
@@ -4025,7 +4043,7 @@
         <v>43587</v>
       </c>
       <c r="B176" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C176">
         <v>100</v>
@@ -4034,7 +4052,7 @@
         <v>5</v>
       </c>
       <c r="E176" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.15">
@@ -4042,7 +4060,7 @@
         <v>43586</v>
       </c>
       <c r="B177" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C177">
         <v>100</v>
@@ -4051,7 +4069,7 @@
         <v>5</v>
       </c>
       <c r="E177" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.15">
@@ -4059,7 +4077,7 @@
         <v>43585</v>
       </c>
       <c r="B178" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C178">
         <v>100</v>
@@ -4068,7 +4086,7 @@
         <v>5</v>
       </c>
       <c r="E178" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.15">
@@ -4076,16 +4094,16 @@
         <v>43584</v>
       </c>
       <c r="B179" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C179">
         <v>200</v>
       </c>
       <c r="D179" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E179" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.15">
@@ -4093,7 +4111,7 @@
         <v>43583</v>
       </c>
       <c r="B180" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C180">
         <v>100</v>
@@ -4102,7 +4120,7 @@
         <v>5</v>
       </c>
       <c r="E180" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.15">
@@ -4110,16 +4128,16 @@
         <v>43582</v>
       </c>
       <c r="B181" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C181">
         <v>300</v>
       </c>
       <c r="D181" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E181" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.15">
@@ -4127,16 +4145,16 @@
         <v>43581</v>
       </c>
       <c r="B182" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C182">
         <v>300</v>
       </c>
       <c r="D182" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E182" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.15">
@@ -4144,7 +4162,7 @@
         <v>43580</v>
       </c>
       <c r="B183" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C183">
         <v>100</v>
@@ -4153,7 +4171,7 @@
         <v>5</v>
       </c>
       <c r="E183" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.15">
@@ -4161,16 +4179,16 @@
         <v>43579</v>
       </c>
       <c r="B184" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C184">
         <v>300</v>
       </c>
       <c r="D184" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E184" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.15">
@@ -4178,7 +4196,7 @@
         <v>43578</v>
       </c>
       <c r="B185" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C185">
         <v>100</v>
@@ -4187,7 +4205,7 @@
         <v>5</v>
       </c>
       <c r="E185" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.15">
@@ -4195,16 +4213,16 @@
         <v>43577</v>
       </c>
       <c r="B186" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C186">
         <v>400</v>
       </c>
       <c r="D186" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E186" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.15">
@@ -4212,7 +4230,7 @@
         <v>43576</v>
       </c>
       <c r="B187" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C187">
         <v>100</v>
@@ -4221,7 +4239,7 @@
         <v>5</v>
       </c>
       <c r="E187" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.15">
@@ -4229,16 +4247,16 @@
         <v>43575</v>
       </c>
       <c r="B188" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C188">
         <v>300</v>
       </c>
       <c r="D188" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E188" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.15">
@@ -4246,16 +4264,16 @@
         <v>43574</v>
       </c>
       <c r="B189" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C189">
         <v>200</v>
       </c>
       <c r="D189" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E189" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.15">
@@ -4263,16 +4281,16 @@
         <v>43573</v>
       </c>
       <c r="B190" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C190">
         <v>300</v>
       </c>
       <c r="D190" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E190" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.15">
@@ -4280,16 +4298,16 @@
         <v>43572</v>
       </c>
       <c r="B191" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C191">
         <v>400</v>
       </c>
       <c r="D191" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E191" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.15">
@@ -4297,7 +4315,7 @@
         <v>43571</v>
       </c>
       <c r="B192" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C192">
         <v>100</v>
@@ -4306,7 +4324,7 @@
         <v>5</v>
       </c>
       <c r="E192" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.15">
@@ -4314,16 +4332,16 @@
         <v>43570</v>
       </c>
       <c r="B193" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C193">
         <v>200</v>
       </c>
       <c r="D193" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E193" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.15">
@@ -4331,16 +4349,16 @@
         <v>43569</v>
       </c>
       <c r="B194" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C194">
         <v>400</v>
       </c>
       <c r="D194" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E194" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.15">
@@ -4348,16 +4366,16 @@
         <v>43568</v>
       </c>
       <c r="B195" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C195">
         <v>200</v>
       </c>
       <c r="D195" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E195" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.15">
@@ -4365,16 +4383,16 @@
         <v>43567</v>
       </c>
       <c r="B196" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C196">
         <v>300</v>
       </c>
       <c r="D196" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E196" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.15">
@@ -4382,16 +4400,16 @@
         <v>43566</v>
       </c>
       <c r="B197" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C197">
         <v>300</v>
       </c>
       <c r="D197" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E197" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.15">
@@ -4399,16 +4417,16 @@
         <v>43565</v>
       </c>
       <c r="B198" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C198">
         <v>200</v>
       </c>
       <c r="D198" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E198" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.15">
@@ -4416,16 +4434,16 @@
         <v>43564</v>
       </c>
       <c r="B199" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C199">
         <v>400</v>
       </c>
       <c r="D199" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E199" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.15">
@@ -4433,16 +4451,16 @@
         <v>43563</v>
       </c>
       <c r="B200" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C200">
         <v>300</v>
       </c>
       <c r="D200" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="E200" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated file names to opmtimize for SEO. German names for german files.
</commit_message>
<xml_diff>
--- a/_templates/Strategic-Logistics-Board/Warehouse_Complaints_en.xlsx
+++ b/_templates/Strategic-Logistics-Board/Warehouse_Complaints_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Strategic-Logistics-Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AD344F-3937-B843-96F0-617681CD01A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C51B462-8F04-394A-BAC2-65D74DD10321}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-52000" yWindow="-3720" windowWidth="42920" windowHeight="28080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="226">
   <si>
     <t>date</t>
   </si>
@@ -698,6 +698,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 2 out of 3 items were incomplete.</t>
+  </si>
+  <si>
+    <t>Don’t forget the wine please. We really need it.</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1054,7 @@
   <dimension ref="A1:E200"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1196,7 +1199,7 @@
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">

</xml_diff>